<commit_message>
before ignoring fixations out of bounds
</commit_message>
<xml_diff>
--- a/localExperiments/pipeSpoolAssembly/ParticipantDataOrdered.xlsx
+++ b/localExperiments/pipeSpoolAssembly/ParticipantDataOrdered.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattsears/code/eyetracker/eyeTrackingData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattsears/code/eyetracker/localExperiments/pipeSpoolAssembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADADEA2-4DB9-F948-B06B-D61182342A93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F77EF77-BF72-8546-9B31-DE8EA0BD1A63}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" xr2:uid="{31EF0B80-0620-B140-B391-1410B2F8110A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19040" xr2:uid="{31EF0B80-0620-B140-B391-1410B2F8110A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +121,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -137,8 +144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,8 +185,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -211,10 +218,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -223,17 +230,18 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,7 +558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H30" sqref="H30"/>
+      <selection pane="topRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>